<commit_message>
10/22 Last commit 修正
</commit_message>
<xml_diff>
--- a/static.xlsx
+++ b/static.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taiyo\Desktop\python\The1\the1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9088608B-2152-407D-8C2D-6B47E8770C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E07064-8739-4F4F-B388-5FF292C43C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{5DF35994-0507-450F-86A4-945F99D90598}"/>
   </bookViews>
@@ -5805,8 +5805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF0D496-3BD6-4FBB-A165-F439C62BEF69}">
   <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
11/2 day2 FINAL COMMIT
</commit_message>
<xml_diff>
--- a/static.xlsx
+++ b/static.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c2aa0dda8f38b74/デスクトップ/BPUMP/The1/the1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="13_ncr:1_{25BF0422-1179-4F11-A350-148A70AF9578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6518E57D-A5F2-4ACF-8061-834EFABE8CC5}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:1_{25BF0422-1179-4F11-A350-148A70AF9578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BB3C31E-B6AB-40F0-9764-1C463689FD7A}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="2" xr2:uid="{5DF35994-0507-450F-86A4-945F99D90598}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" firstSheet="2" activeTab="6" xr2:uid="{5DF35994-0507-450F-86A4-945F99D90598}"/>
   </bookViews>
   <sheets>
     <sheet name="asp_men" sheetId="5" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="231">
   <si>
     <t>FUN2</t>
     <phoneticPr fontId="1"/>
@@ -521,39 +521,6 @@
     <t>Mao NAKAMURA</t>
   </si>
   <si>
-    <t>kessyou 1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>kessyou 2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>kessyou 3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>kessyou 4</t>
-  </si>
-  <si>
-    <t>kessyou 5</t>
-  </si>
-  <si>
-    <t>kessyou 6</t>
-  </si>
-  <si>
-    <t>kessyou 7</t>
-  </si>
-  <si>
-    <t>kessyou 8</t>
-  </si>
-  <si>
-    <t>kessyou 9</t>
-  </si>
-  <si>
-    <t>kessyou 10</t>
-  </si>
-  <si>
     <t>Yarden CHARNY</t>
   </si>
   <si>
@@ -835,6 +802,38 @@
   </si>
   <si>
     <t>Mashiro KUZUU</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Melody SEKIKAWA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mao NAKAMURA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Meini LI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sorato ANRAKU</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dohyun LEE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Yusuke SUGIMOTO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Yufei PAN</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rei SUGIMOTO</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1638,7 +1637,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="9"/>
@@ -1648,7 +1647,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -1658,7 +1657,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -1671,7 +1670,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="9"/>
@@ -1681,7 +1680,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -1692,7 +1691,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -1703,7 +1702,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="9"/>
@@ -1714,7 +1713,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -1724,7 +1723,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -1734,7 +1733,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="9"/>
@@ -1744,7 +1743,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -1754,7 +1753,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1764,7 +1763,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="9"/>
@@ -1774,7 +1773,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -1784,7 +1783,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -1794,7 +1793,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="9"/>
@@ -1804,7 +1803,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1814,7 +1813,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -1824,7 +1823,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -1834,7 +1833,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1844,7 +1843,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -1854,7 +1853,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -1864,7 +1863,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -1874,7 +1873,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -1884,7 +1883,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -1894,7 +1893,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -1904,7 +1903,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -1914,7 +1913,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -1924,7 +1923,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -1934,7 +1933,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -1944,7 +1943,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -1954,7 +1953,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -1964,7 +1963,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -1974,7 +1973,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -1984,7 +1983,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -1994,7 +1993,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -2933,7 +2932,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="9"/>
@@ -2943,7 +2942,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -2953,7 +2952,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -2966,7 +2965,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="9"/>
@@ -2976,7 +2975,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -2987,7 +2986,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -2998,7 +2997,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="9"/>
@@ -3009,7 +3008,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -3019,7 +3018,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -3029,7 +3028,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="9"/>
@@ -3039,7 +3038,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -4158,7 +4157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C653A833-BC96-46FB-AD28-C9B05ABD08B5}">
   <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -4178,7 +4177,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D1" s="9"/>
     </row>
@@ -4187,7 +4186,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -4197,7 +4196,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -4210,7 +4209,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="9"/>
@@ -4220,7 +4219,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -4231,7 +4230,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -4263,7 +4262,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -4364,7 +4363,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -4374,7 +4373,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -5454,7 +5453,7 @@
   <dimension ref="A1:I144"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
@@ -5473,7 +5472,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="9"/>
@@ -5483,7 +5482,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -5493,7 +5492,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -5506,7 +5505,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="9"/>
@@ -5516,7 +5515,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -5527,7 +5526,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -5609,7 +5608,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -5639,7 +5638,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -5649,7 +5648,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -6768,7 +6767,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="9"/>
@@ -6778,7 +6777,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -6788,7 +6787,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -6801,7 +6800,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="9"/>
@@ -6811,7 +6810,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -6822,7 +6821,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -6833,7 +6832,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="9"/>
@@ -6844,7 +6843,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -7703,7 +7702,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="9"/>
@@ -7713,7 +7712,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -7723,7 +7722,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -7736,7 +7735,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="9"/>
@@ -7746,7 +7745,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -7757,7 +7756,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -7768,7 +7767,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="9"/>
@@ -7779,7 +7778,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -8618,8 +8617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB51AC29-8C4E-A243-8D29-DA52D2852FA3}">
   <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
@@ -8638,7 +8637,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>131</v>
+        <v>226</v>
       </c>
       <c r="D1" s="9"/>
     </row>
@@ -8647,7 +8646,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>132</v>
+        <v>227</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -8657,7 +8656,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>133</v>
+        <v>216</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -8670,7 +8669,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>134</v>
+        <v>228</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="9"/>
@@ -8680,7 +8679,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>135</v>
+        <v>229</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -8691,7 +8690,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>136</v>
+        <v>230</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -8702,7 +8701,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="9"/>
@@ -8713,7 +8712,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -8723,7 +8722,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -8733,7 +8732,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="9"/>
@@ -9554,7 +9553,7 @@
   <dimension ref="A1:I144"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B11" sqref="B7:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
@@ -9573,7 +9572,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>131</v>
+        <v>223</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="9"/>
@@ -9583,7 +9582,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>132</v>
+        <v>224</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -9593,7 +9592,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>133</v>
+        <v>218</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -9606,7 +9605,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>134</v>
+        <v>225</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="9"/>
@@ -9616,7 +9615,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -9626,8 +9625,8 @@
       <c r="A6" s="9">
         <v>6</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>136</v>
+      <c r="B6" s="15" t="s">
+        <v>127</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -9638,7 +9637,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="9"/>
@@ -9649,7 +9648,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -9659,7 +9658,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -9669,7 +9668,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="9"/>
@@ -10672,7 +10671,7 @@
       <c r="C13" s="10"/>
       <c r="D13" s="9"/>
       <c r="G13" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="H13" t="str">
         <f>RIGHT(G13, LEN(G13)-FIND(" ", G13))</f>
@@ -10693,7 +10692,7 @@
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="G14" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" ref="H14:I23" si="0">RIGHT(G14, LEN(G14)-FIND(" ", G14))</f>
@@ -10714,7 +10713,7 @@
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="G15" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -10735,7 +10734,7 @@
       <c r="C16" s="10"/>
       <c r="D16" s="9"/>
       <c r="G16" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -10756,7 +10755,7 @@
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="G17" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -10777,7 +10776,7 @@
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="G18" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -10798,7 +10797,7 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="G19" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -10819,7 +10818,7 @@
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="G20" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -10840,7 +10839,7 @@
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="G21" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -10861,7 +10860,7 @@
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="G22" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -10882,7 +10881,7 @@
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="G23" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -10903,7 +10902,7 @@
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="G24" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" ref="H24:I24" si="1">RIGHT(G24, LEN(G24)-FIND(" ", G24))</f>
@@ -10924,7 +10923,7 @@
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="G25" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" ref="H25:I25" si="2">RIGHT(G25, LEN(G25)-FIND(" ", G25))</f>
@@ -10945,7 +10944,7 @@
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="G26" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" ref="H26:I26" si="3">RIGHT(G26, LEN(G26)-FIND(" ", G26))</f>
@@ -10966,7 +10965,7 @@
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="G27" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" ref="H27:I27" si="4">RIGHT(G27, LEN(G27)-FIND(" ", G27))</f>
@@ -10987,7 +10986,7 @@
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="G28" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" ref="H28:I28" si="5">RIGHT(G28, LEN(G28)-FIND(" ", G28))</f>
@@ -11008,7 +11007,7 @@
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="G29" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" ref="H29:I29" si="6">RIGHT(G29, LEN(G29)-FIND(" ", G29))</f>
@@ -11029,7 +11028,7 @@
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="G30" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" ref="H30:I30" si="7">RIGHT(G30, LEN(G30)-FIND(" ", G30))</f>
@@ -11050,7 +11049,7 @@
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="G31" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" ref="H31:I31" si="8">RIGHT(G31, LEN(G31)-FIND(" ", G31))</f>
@@ -11071,7 +11070,7 @@
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="G32" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" ref="H32:I32" si="9">RIGHT(G32, LEN(G32)-FIND(" ", G32))</f>
@@ -11092,7 +11091,7 @@
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="G33" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" ref="H33:I33" si="10">RIGHT(G33, LEN(G33)-FIND(" ", G33))</f>
@@ -11113,7 +11112,7 @@
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="G34" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" ref="H34:I34" si="11">RIGHT(G34, LEN(G34)-FIND(" ", G34))</f>
@@ -11134,7 +11133,7 @@
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="G35" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" ref="H35:I35" si="12">RIGHT(G35, LEN(G35)-FIND(" ", G35))</f>
@@ -11155,7 +11154,7 @@
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="G36" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" ref="H36:I36" si="13">RIGHT(G36, LEN(G36)-FIND(" ", G36))</f>
@@ -11176,7 +11175,7 @@
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="G37" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" ref="H37:I37" si="14">RIGHT(G37, LEN(G37)-FIND(" ", G37))</f>
@@ -11197,7 +11196,7 @@
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="G38" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" ref="H38:I38" si="15">RIGHT(G38, LEN(G38)-FIND(" ", G38))</f>
@@ -11218,7 +11217,7 @@
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="G39" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" ref="H39:I39" si="16">RIGHT(G39, LEN(G39)-FIND(" ", G39))</f>
@@ -11239,7 +11238,7 @@
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="G40" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" ref="H40:I40" si="17">RIGHT(G40, LEN(G40)-FIND(" ", G40))</f>
@@ -11260,7 +11259,7 @@
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="G41" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" ref="H41:I41" si="18">RIGHT(G41, LEN(G41)-FIND(" ", G41))</f>
@@ -11281,7 +11280,7 @@
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="G42" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" ref="H42" si="19">RIGHT(G42, LEN(G42)-FIND(" ", G42))</f>
@@ -11302,7 +11301,7 @@
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="G43" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" ref="H43:I43" si="21">RIGHT(G43, LEN(G43)-FIND(" ", G43))</f>
@@ -11323,7 +11322,7 @@
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="G44" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" ref="H44:I44" si="22">RIGHT(G44, LEN(G44)-FIND(" ", G44))</f>
@@ -11344,7 +11343,7 @@
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
       <c r="G45" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" ref="H45:I45" si="23">RIGHT(G45, LEN(G45)-FIND(" ", G45))</f>
@@ -11365,7 +11364,7 @@
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="G46" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" ref="H46:I46" si="24">RIGHT(G46, LEN(G46)-FIND(" ", G46))</f>
@@ -11386,7 +11385,7 @@
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="G47" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" ref="H47:I47" si="25">RIGHT(G47, LEN(G47)-FIND(" ", G47))</f>
@@ -11407,7 +11406,7 @@
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="G48" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" ref="H48:I48" si="26">RIGHT(G48, LEN(G48)-FIND(" ", G48))</f>

</xml_diff>